<commit_message>
Subo el product JSON y traslado las imagenes a Public/images
</commit_message>
<xml_diff>
--- a/Pre-produccion/Productos.xlsx
+++ b/Pre-produccion/Productos.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nahue\Documents\DH\Goodbike\grupo_1_GoodBikes\BACKUP HTML\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nahue\Documents\DH\Goodbike\grupo_1_GoodBikes\Pre-produccion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03ECE77B-4E47-4D4C-8B89-8F2B4CB5A2D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053E26E3-AD49-4E81-8972-F14DF8254C30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{27B5C772-8F59-43EF-B2A7-008967AF63AC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{27B5C772-8F59-43EF-B2A7-008967AF63AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="197">
   <si>
     <t>ID</t>
   </si>
@@ -325,6 +327,306 @@
   </si>
   <si>
     <t>Categoria</t>
+  </si>
+  <si>
+    <t>"1"</t>
+  </si>
+  <si>
+    <t>"Bicicleta"</t>
+  </si>
+  <si>
+    <t>"Mountain Bike Firebird R29 Doble suspensión"</t>
+  </si>
+  <si>
+    <t>"Firebird"</t>
+  </si>
+  <si>
+    <t>"R29 Doble suspensión"</t>
+  </si>
+  <si>
+    <t>"Género: Unisex, Material del cuadro: Acero, Número de cambios: 21, Tipo de freno: Disco mecánico, Suspensión: Doble, Rodado: 29, Modelo: DobSusRodado29, Tipo: Mountain Bike, Manubrio: Acero, Pedal: Plástico, Peso: 15 kg, Origen: China, Garantía del proveedor: 3 meses, Requiere armado: Sí, Info Adicional: No"</t>
+  </si>
+  <si>
+    <t>"FireBird-doble-suspension-R29.jpeg"</t>
+  </si>
+  <si>
+    <t>"71999"</t>
+  </si>
+  <si>
+    <t>"50"</t>
+  </si>
+  <si>
+    <t>"2"</t>
+  </si>
+  <si>
+    <t>"Todoterreno Aurora Bacota"</t>
+  </si>
+  <si>
+    <t>"Aurora"</t>
+  </si>
+  <si>
+    <t>"Bacota"</t>
+  </si>
+  <si>
+    <t>"Género: Unisex, Material del cuadro: Aluminio, Número de cambios: 7, Tipo de freno: Disco mecánico Shimano, Suspensión: Doble, Rodado: Especial 26x4, Modelo: Bacota, Tipo: Mountain Bike, Manubrio: Chopero Acero, Pedal: Acero, Peso: 9 Kg, Origen: China, Garantía del proveedor: 6 meses, Requiere armado: Sí, Info Adicional: Ruedas ultraresistentes que previenen pinchaduras"</t>
+  </si>
+  <si>
+    <t>"Aurora-bacota.jpg"</t>
+  </si>
+  <si>
+    <t>"98000"</t>
+  </si>
+  <si>
+    <t>"30"</t>
+  </si>
+  <si>
+    <t>"3"</t>
+  </si>
+  <si>
+    <t>"Mountain Kike Teknial Tarpan 100er"</t>
+  </si>
+  <si>
+    <t>"Teknial"</t>
+  </si>
+  <si>
+    <t>"Tarpan 100er"</t>
+  </si>
+  <si>
+    <t>"Género: Hombre, Material del cuadro: Aluminio, Número de cambios: 21, Tipo de freno: Disco mecánico Shimano, Suspensión: Simple, Rodado: 29, Modelo: Tarpan, Tipo: Mountain Bike, Manubrio: Acero MTB, Pedal: Plásticos, Peso: 14 kg, Origen: China, Garantía del proveedor: 12 meses, Requiere armado: No, Info Adicional: No"</t>
+  </si>
+  <si>
+    <t>"mountain-bike-teknial-tarpan-100er-2021.jpg"</t>
+  </si>
+  <si>
+    <t>"52000"</t>
+  </si>
+  <si>
+    <t>"4"</t>
+  </si>
+  <si>
+    <t>"Eléctrica plegable Ride Daily 250W 13AH"</t>
+  </si>
+  <si>
+    <t>"Ride Daily"</t>
+  </si>
+  <si>
+    <t>"ID V"</t>
+  </si>
+  <si>
+    <t>"Género: Unisex, Material del cuadro: Aluminio, Número de cambios: 6, Tipo de freno: Disco mecánico, Suspensión: Delantera, Rodado: 20, Modelo: ID V, Tipo: Eléctrica, Manubrio: Aluminio, Pedal: Plástico, Peso: 15 kg, Origen: Origen, Garantía del proveedor: 2 años, Requiere armado: No, Info Adicional: Motor 250Wh 8FUN japonés Batería SAMSUNG 13AH : 60km de autonomía. Sistema de asistencia al pedaleo, velocidad máxima limitada segun la ley a 25km/h"</t>
+  </si>
+  <si>
+    <t>"Ride-Daily-250W-13AH.jpeg"</t>
+  </si>
+  <si>
+    <t>"248800"</t>
+  </si>
+  <si>
+    <t>"5"</t>
+  </si>
+  <si>
+    <t>"Playera Randers BKE-001"</t>
+  </si>
+  <si>
+    <t>"RANDERS"</t>
+  </si>
+  <si>
+    <t>"BKE-001"</t>
+  </si>
+  <si>
+    <t>"Género: Unisex, Material del cuadro: Acero, Número de cambios: Sin cambios, Tipo de freno: Contrapedal, Suspensión: Sin suspensión, Rodado: 26, Modelo: BKE-001-B, Tipo: Urbana, Manubrio: Acero, Pedal: Plástico, Peso: 14 kg, Origen: Argentina, Garantía del proveedor: 6 meses, Requiere armado: No, Info Adicional: No"</t>
+  </si>
+  <si>
+    <t>"Playera-Randers-BKE-001.jpg"</t>
+  </si>
+  <si>
+    <t>"28000"</t>
+  </si>
+  <si>
+    <t>"ID":</t>
+  </si>
+  <si>
+    <t>"Categoria":</t>
+  </si>
+  <si>
+    <t>"Titulo":</t>
+  </si>
+  <si>
+    <t>"Marca":</t>
+  </si>
+  <si>
+    <t>"Modelo":</t>
+  </si>
+  <si>
+    <t>"Detalles":</t>
+  </si>
+  <si>
+    <t>"Imagen":</t>
+  </si>
+  <si>
+    <t>"Precio":</t>
+  </si>
+  <si>
+    <t>"Cantidad":</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>"20"</t>
+  </si>
+  <si>
+    <t>"ID":"1",</t>
+  </si>
+  <si>
+    <t>"Categoria":"Bicicleta",</t>
+  </si>
+  <si>
+    <t>"Titulo":"Mountain Bike Firebird R29 Doble suspensión",</t>
+  </si>
+  <si>
+    <t>"Marca":"Firebird",</t>
+  </si>
+  <si>
+    <t>"Modelo":"R29 Doble suspensión",</t>
+  </si>
+  <si>
+    <t>"Detalles":"Género: Unisex, Material del cuadro: Acero, Número de cambios: 21, Tipo de freno: Disco mecánico, Suspensión: Doble, Rodado: 29, Modelo: DobSusRodado29, Tipo: Mountain Bike, Manubrio: Acero, Pedal: Plástico, Peso: 15 kg, Origen: China, Garantía del proveedor: 3 meses, Requiere armado: Sí, Info Adicional: No",</t>
+  </si>
+  <si>
+    <t>"Imagen":"FireBird-doble-suspension-R29.jpeg",</t>
+  </si>
+  <si>
+    <t>"Precio":"71999",</t>
+  </si>
+  <si>
+    <t>"Cantidad":"50"</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>"ID":"2",</t>
+  </si>
+  <si>
+    <t>"Titulo":"Todoterreno Aurora Bacota",</t>
+  </si>
+  <si>
+    <t>"Marca":"Aurora",</t>
+  </si>
+  <si>
+    <t>"Modelo":"Bacota",</t>
+  </si>
+  <si>
+    <t>"Detalles":"Género: Unisex, Material del cuadro: Aluminio, Número de cambios: 7, Tipo de freno: Disco mecánico Shimano, Suspensión: Doble, Rodado: Especial 26x4, Modelo: Bacota, Tipo: Mountain Bike, Manubrio: Chopero Acero, Pedal: Acero, Peso: 9 Kg, Origen: China, Garantía del proveedor: 6 meses, Requiere armado: Sí, Info Adicional: Ruedas ultraresistentes que previenen pinchaduras",</t>
+  </si>
+  <si>
+    <t>"Imagen":"Aurora-bacota.jpg",</t>
+  </si>
+  <si>
+    <t>"Precio":"98000",</t>
+  </si>
+  <si>
+    <t>"Cantidad":"30"</t>
+  </si>
+  <si>
+    <t>"ID":"3",</t>
+  </si>
+  <si>
+    <t>"Titulo":"Mountain Kike Teknial Tarpan 100er",</t>
+  </si>
+  <si>
+    <t>"Marca":"Teknial",</t>
+  </si>
+  <si>
+    <t>"Modelo":"Tarpan 100er",</t>
+  </si>
+  <si>
+    <t>"Detalles":"Género: Hombre, Material del cuadro: Aluminio, Número de cambios: 21, Tipo de freno: Disco mecánico Shimano, Suspensión: Simple, Rodado: 29, Modelo: Tarpan, Tipo: Mountain Bike, Manubrio: Acero MTB, Pedal: Plásticos, Peso: 14 kg, Origen: China, Garantía del proveedor: 12 meses, Requiere armado: No, Info Adicional: No",</t>
+  </si>
+  <si>
+    <t>"Imagen":"mountain-bike-teknial-tarpan-100er-2021.jpg",</t>
+  </si>
+  <si>
+    <t>"Precio":"52000",</t>
+  </si>
+  <si>
+    <t>"ID":"4",</t>
+  </si>
+  <si>
+    <t>"Titulo":"Eléctrica plegable Ride Daily 250W 13AH",</t>
+  </si>
+  <si>
+    <t>"Marca":"Ride Daily",</t>
+  </si>
+  <si>
+    <t>"Modelo":"ID V",</t>
+  </si>
+  <si>
+    <t>"Detalles":"Género: Unisex, Material del cuadro: Aluminio, Número de cambios: 6, Tipo de freno: Disco mecánico, Suspensión: Delantera, Rodado: 20, Modelo: ID V, Tipo: Eléctrica, Manubrio: Aluminio, Pedal: Plástico, Peso: 15 kg, Origen: Origen, Garantía del proveedor: 2 años, Requiere armado: No, Info Adicional: Motor 250Wh 8FUN japonés Batería SAMSUNG 13AH : 60km de autonomía. Sistema de asistencia al pedaleo, velocidad máxima limitada segun la ley a 25km/h",</t>
+  </si>
+  <si>
+    <t>"Imagen":"Ride-Daily-250W-13AH.jpeg",</t>
+  </si>
+  <si>
+    <t>"Precio":"248800",</t>
+  </si>
+  <si>
+    <t>"Cantidad":"20"</t>
+  </si>
+  <si>
+    <t>"ID":"5",</t>
+  </si>
+  <si>
+    <t>"Titulo":"Playera Randers BKE-001",</t>
+  </si>
+  <si>
+    <t>"Marca":"RANDERS",</t>
+  </si>
+  <si>
+    <t>"Modelo":"BKE-001",</t>
+  </si>
+  <si>
+    <t>"Detalles":"Género: Unisex, Material del cuadro: Acero, Número de cambios: Sin cambios, Tipo de freno: Contrapedal, Suspensión: Sin suspensión, Rodado: 26, Modelo: BKE-001-B, Tipo: Urbana, Manubrio: Acero, Pedal: Plástico, Peso: 14 kg, Origen: Argentina, Garantía del proveedor: 6 meses, Requiere armado: No, Info Adicional: No",</t>
+  </si>
+  <si>
+    <t>"Imagen":"Playera-Randers-BKE-001.jpg",</t>
+  </si>
+  <si>
+    <t>"Precio":"28000",</t>
+  </si>
+  <si>
+    <t>"ID":1,</t>
+  </si>
+  <si>
+    <t>"ID":2,</t>
+  </si>
+  <si>
+    <t>"ID":3,</t>
+  </si>
+  <si>
+    <t>"ID":4,</t>
+  </si>
+  <si>
+    <t>"ID":5,</t>
+  </si>
+  <si>
+    <t>"Cantidad":20</t>
+  </si>
+  <si>
+    <t>"Cantidad":50</t>
+  </si>
+  <si>
+    <t>"Cantidad":30</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t>},</t>
+  </si>
+  <si>
+    <t>}</t>
   </si>
 </sst>
 </file>
@@ -412,7 +714,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -435,6 +737,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1160,7 +1465,7 @@
         <v>16</v>
       </c>
       <c r="G19" t="str">
-        <f>+E19&amp;": "&amp;F19</f>
+        <f t="shared" ref="G19:G26" si="0">+E19&amp;": "&amp;F19</f>
         <v>Género: Unisex</v>
       </c>
     </row>
@@ -1179,7 +1484,7 @@
         <v>18</v>
       </c>
       <c r="G20" t="str">
-        <f>+E20&amp;": "&amp;F20</f>
+        <f t="shared" si="0"/>
         <v>Material del cuadro: Aluminio</v>
       </c>
       <c r="J20" t="s">
@@ -1201,7 +1506,7 @@
         <v>7</v>
       </c>
       <c r="G21" t="str">
-        <f>+E21&amp;": "&amp;F21</f>
+        <f t="shared" si="0"/>
         <v>Número de cambios: 7</v>
       </c>
     </row>
@@ -1220,7 +1525,7 @@
         <v>21</v>
       </c>
       <c r="G22" t="str">
-        <f>+E22&amp;": "&amp;F22</f>
+        <f t="shared" si="0"/>
         <v>Tipo de freno: Disco mecánico</v>
       </c>
     </row>
@@ -1239,7 +1544,7 @@
         <v>23</v>
       </c>
       <c r="G23" t="str">
-        <f>+E23&amp;": "&amp;F23</f>
+        <f t="shared" si="0"/>
         <v>Suspensión: Delantera</v>
       </c>
     </row>
@@ -1258,7 +1563,7 @@
         <v>16</v>
       </c>
       <c r="G24" t="str">
-        <f>+E24&amp;": "&amp;F24</f>
+        <f t="shared" si="0"/>
         <v>Rodado: 16</v>
       </c>
     </row>
@@ -1277,7 +1582,7 @@
         <v>86</v>
       </c>
       <c r="G25" t="str">
-        <f>+E25&amp;": "&amp;F25</f>
+        <f t="shared" si="0"/>
         <v>Modelo: Trimove CJ</v>
       </c>
     </row>
@@ -1296,11 +1601,11 @@
         <v>27</v>
       </c>
       <c r="G26" t="str">
-        <f>+E26&amp;": "&amp;F26</f>
+        <f t="shared" si="0"/>
         <v>Tipo: Eléctrica</v>
       </c>
     </row>
-    <row r="27" spans="2:10" ht="28" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B27" s="3" t="s">
         <v>28</v>
       </c>
@@ -1315,7 +1620,7 @@
         <v>18</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" ref="G27:G33" si="0">+E27&amp;": "&amp;F27</f>
+        <f t="shared" ref="G27:G33" si="1">+E27&amp;": "&amp;F27</f>
         <v>Manubrio: Aluminio</v>
       </c>
     </row>
@@ -1334,7 +1639,7 @@
         <v>18</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Pedal: Aluminio</v>
       </c>
     </row>
@@ -1353,7 +1658,7 @@
         <v>87</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Peso: 18 kg</v>
       </c>
     </row>
@@ -1372,7 +1677,7 @@
         <v>42</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Origen: China</v>
       </c>
     </row>
@@ -1391,7 +1696,7 @@
         <v>35</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Garantía del proveedor: 6 meses</v>
       </c>
     </row>
@@ -1410,7 +1715,7 @@
         <v>37</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Requiere armado: No</v>
       </c>
     </row>
@@ -1429,11 +1734,11 @@
         <v>88</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Info Adicional: Batería Litio Ion</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="42" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:7" ht="28" x14ac:dyDescent="0.35">
       <c r="B34" s="5" t="s">
         <v>36</v>
       </c>
@@ -1505,15 +1810,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8CBAE45-D0FE-4384-8201-DA5BE3C68130}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="7" max="7" width="39" customWidth="1"/>
+    <col min="9" max="9" width="14.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
@@ -1544,9 +1850,6 @@
       <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" t="s">
-        <v>68</v>
-      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
@@ -1576,9 +1879,6 @@
       <c r="I2">
         <v>50</v>
       </c>
-      <c r="J2" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
@@ -1608,9 +1908,7 @@
       <c r="I3">
         <v>30</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>69</v>
-      </c>
+      <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -1640,9 +1938,6 @@
       <c r="I4">
         <v>50</v>
       </c>
-      <c r="J4" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -1672,9 +1967,6 @@
       <c r="I5">
         <v>5</v>
       </c>
-      <c r="J5" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
@@ -1704,9 +1996,6 @@
       <c r="I6">
         <v>50</v>
       </c>
-      <c r="J6" t="s">
-        <v>62</v>
-      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
@@ -1736,9 +2025,6 @@
       <c r="I7">
         <v>100</v>
       </c>
-      <c r="J7" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
@@ -1768,9 +2054,6 @@
       <c r="I8">
         <v>10</v>
       </c>
-      <c r="J8" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
@@ -1800,9 +2083,7 @@
       <c r="I9">
         <v>50</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
@@ -1832,9 +2113,6 @@
       <c r="I10">
         <v>50</v>
       </c>
-      <c r="J10" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
@@ -1864,19 +2142,1387 @@
       <c r="I11">
         <v>10</v>
       </c>
-      <c r="J11" t="s">
-        <v>94</v>
-      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="9"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C14" s="9"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>137</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="9"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="9"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" s="9"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" s="9"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>141</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" s="9"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="9"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>143</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" s="9"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>136</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" s="9"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>137</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="9"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" s="9"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>139</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="9"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>140</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" s="9"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" s="9"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>142</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" s="9"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30" s="9"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>135</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31" s="9"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>136</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" s="9"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>137</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" s="9"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>138</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" s="9"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>139</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" s="9"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>140</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="9"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>141</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" s="9"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>142</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" s="9"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>143</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" s="9"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>135</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C40" s="9"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>136</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41" s="9"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>137</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" s="9"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>138</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C43" s="9"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>139</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C44" s="9"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>140</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C45" s="9"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>141</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C46" s="9"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>142</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C47" s="9"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>143</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C48" s="9"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>135</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C49" s="9"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>136</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C50" s="9"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>137</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C51" s="9"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>138</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C52" s="9"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>139</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C53" s="9"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>140</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C54" s="9"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>141</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C55" s="9"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>142</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C56" s="9"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>143</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C57" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D9" r:id="rId1" display="https://www.falabella.com.ar/falabella-ar/search?Ntt=&amp;f.product.brandName=Randers" xr:uid="{5471F893-6454-4D8D-8457-065188BE2414}"/>
-    <hyperlink ref="J2" r:id="rId2" xr:uid="{07B7E752-93B7-4427-A780-4086997691B7}"/>
-    <hyperlink ref="D8" r:id="rId3" display="https://www.falabella.com.ar/falabella-ar/search?Ntt=&amp;f.product.brandName=Raleigh" xr:uid="{954DA124-D74A-4066-BE1E-00E8C39CA472}"/>
-    <hyperlink ref="D6" r:id="rId4" display="https://www.falabella.com.ar/falabella-ar/search?Ntt=&amp;f.product.brandName=Randers" xr:uid="{8B8270AA-232E-420E-BEA8-090A8654C27C}"/>
-    <hyperlink ref="J3" r:id="rId5" xr:uid="{60378AB9-1C8E-4B92-A673-CC0818D77455}"/>
-    <hyperlink ref="J9" r:id="rId6" xr:uid="{5B8CAAD4-C13D-43A4-B9E8-61F84424F160}"/>
+    <hyperlink ref="D8" r:id="rId2" display="https://www.falabella.com.ar/falabella-ar/search?Ntt=&amp;f.product.brandName=Raleigh" xr:uid="{954DA124-D74A-4066-BE1E-00E8C39CA472}"/>
+    <hyperlink ref="D6" r:id="rId3" display="https://www.falabella.com.ar/falabella-ar/search?Ntt=&amp;f.product.brandName=Randers" xr:uid="{8B8270AA-232E-420E-BEA8-090A8654C27C}"/>
+    <hyperlink ref="B52" r:id="rId4" display="https://www.falabella.com.ar/falabella-ar/search?Ntt=&amp;f.product.brandName=Randers" xr:uid="{3622B9E0-C1B1-4184-A836-68717E65426F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391FA9A3-B86F-40BD-9BBA-0293F83DD0D4}">
+  <dimension ref="B1:E49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E12" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E13" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E14" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E15" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>140</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E16" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>143</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>135</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>136</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E22" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>137</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E23" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>138</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E24" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E25" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>140</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E26" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>141</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E27" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>142</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E28" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>143</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="9"/>
+      <c r="E29" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>135</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E31" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>136</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E32" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>137</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E33" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>138</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E34" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>139</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E35" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>140</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E36" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>141</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E37" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>143</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D39" s="9"/>
+      <c r="E39" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>135</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E41" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>136</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E42" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>137</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E43" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>138</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E44" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>139</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E45" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>140</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E46" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>141</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E47" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>142</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E48" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
+        <v>143</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D49" s="9"/>
+      <c r="E49" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C44" r:id="rId1" display="https://www.falabella.com.ar/falabella-ar/search?Ntt=&amp;f.product.brandName=Randers" xr:uid="{11F1797E-90CC-4EDF-9ABA-4057632FA888}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D05F217-1367-4135-A070-9C83C06545A7}">
+  <dimension ref="A1:B55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>194</v>
+      </c>
+      <c r="B12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>194</v>
+      </c>
+      <c r="B23" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>194</v>
+      </c>
+      <c r="B34" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>194</v>
+      </c>
+      <c r="B45" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B50" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B51" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B52" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B53" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B54" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>196</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>